<commit_message>
Added AS4 profile v2 identifier
</commit_message>
<xml_diff>
--- a/Code Lists/PEPPOL Code Lists - Transport profiles v3.xlsx
+++ b/Code Lists/PEPPOL Code Lists - Transport profiles v3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="110" windowWidth="18920" windowHeight="12300"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="18915" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Transport Profile" sheetId="5" r:id="rId1"/>
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Transport Profile'!$A$1:$F$4</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Profile ID</t>
   </si>
@@ -65,13 +65,22 @@
   </si>
   <si>
     <t>Deprecated since?</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>peppol-transport-as4-v2_0</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,26 +572,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.453125" style="7"/>
+    <col min="5" max="5" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1">
+    <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -602,7 +611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -623,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -640,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -654,6 +663,27 @@
         <v>14</v>
       </c>
       <c r="E4" s="3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>